<commit_message>
primer filtro (Moderadores Conectado)
</commit_message>
<xml_diff>
--- a/Areas.xlsx
+++ b/Areas.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danch\OneDrive\Escritorio\9°\Auditoria\Proyecto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danch\OneDrive\Escritorio\9°\Auditoria\Proyecto\ProyectoModeradores\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DCE2EDAB-C442-4A64-B35D-5B8A1850EC44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A52625BA-9D34-41EA-84D2-D504D7F003C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{9AF59F69-C47A-4E44-91ED-A4453B71C3F7}"/>
+    <workbookView xWindow="3075" yWindow="3075" windowWidth="15375" windowHeight="7725" xr2:uid="{9AF59F69-C47A-4E44-91ED-A4453B71C3F7}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -438,7 +438,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
resolviendo errores de altas en moderadores
</commit_message>
<xml_diff>
--- a/Areas.xlsx
+++ b/Areas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danch\OneDrive\Escritorio\9°\Auditoria\Proyecto\ProyectoModeradores\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A52625BA-9D34-41EA-84D2-D504D7F003C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF4F32BD-9A66-4FA6-820A-B4A177707D72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3075" yWindow="3075" windowWidth="15375" windowHeight="7725" xr2:uid="{9AF59F69-C47A-4E44-91ED-A4453B71C3F7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{9AF59F69-C47A-4E44-91ED-A4453B71C3F7}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -41,49 +41,49 @@
     <t>Codigo</t>
   </si>
   <si>
-    <t>Área IV:</t>
-  </si>
-  <si>
     <t>Humanidades y Ciencias de la Conducta</t>
   </si>
   <si>
     <t>Área III</t>
   </si>
   <si>
-    <t>: Medicina y Salud</t>
-  </si>
-  <si>
     <t>Área II:</t>
   </si>
   <si>
     <t>Biología y Química</t>
   </si>
   <si>
-    <t>Área V:</t>
-  </si>
-  <si>
     <t>Sociales y Económicas</t>
   </si>
   <si>
     <t>Área VII</t>
   </si>
   <si>
-    <t>: Ingeniería e Industria</t>
-  </si>
-  <si>
-    <t>Área VI:</t>
-  </si>
-  <si>
     <t>Biotecnología y Ciencias Agropecuarias</t>
   </si>
   <si>
-    <t>Área I:</t>
-  </si>
-  <si>
     <t>Física, Matemáticas y Ciencias de la Tierra</t>
   </si>
   <si>
     <t>Description</t>
+  </si>
+  <si>
+    <t>Área IV</t>
+  </si>
+  <si>
+    <t>Área V</t>
+  </si>
+  <si>
+    <t>Área VI</t>
+  </si>
+  <si>
+    <t>Área I</t>
+  </si>
+  <si>
+    <t>Medicina y Salud</t>
+  </si>
+  <si>
+    <t>Ingeniería e Industria</t>
   </si>
 </sst>
 </file>
@@ -438,7 +438,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -452,55 +452,55 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
         <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -508,7 +508,7 @@
         <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>